<commit_message>
Versión 6.0 - Actualización datos de Tabita
Actualización de los estados con la información de Tabita
</commit_message>
<xml_diff>
--- a/Resources/data/Versión_6.0/Retorno a la presencialidad_ Estados 2021 FINAL.xlsx
+++ b/Resources/data/Versión_6.0/Retorno a la presencialidad_ Estados 2021 FINAL.xlsx
@@ -18718,7 +18718,7 @@
   <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A8" sqref="$A8:$XFD8"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -18804,7 +18804,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="3" s="75" customFormat="1" ht="25" customHeight="1" spans="1:14">
+    <row r="3" s="75" customFormat="1" ht="25" hidden="1" customHeight="1" spans="1:14">
       <c r="A3" s="82" t="s">
         <v>352</v>
       </c>
@@ -18848,7 +18848,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="4" s="75" customFormat="1" ht="25" customHeight="1" spans="1:14">
+    <row r="4" s="75" customFormat="1" ht="25" hidden="1" customHeight="1" spans="1:14">
       <c r="A4" s="82" t="s">
         <v>352</v>
       </c>
@@ -18892,7 +18892,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="5" s="75" customFormat="1" ht="25" customHeight="1" spans="1:14">
+    <row r="5" s="75" customFormat="1" ht="25" hidden="1" customHeight="1" spans="1:14">
       <c r="A5" s="82" t="s">
         <v>352</v>
       </c>
@@ -18936,7 +18936,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="6" s="75" customFormat="1" ht="25" customHeight="1" spans="1:14">
+    <row r="6" s="75" customFormat="1" ht="25" hidden="1" customHeight="1" spans="1:14">
       <c r="A6" s="82" t="s">
         <v>352</v>
       </c>
@@ -18980,7 +18980,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="7" s="75" customFormat="1" ht="25" customHeight="1" spans="1:14">
+    <row r="7" s="75" customFormat="1" ht="25" hidden="1" customHeight="1" spans="1:14">
       <c r="A7" s="82" t="s">
         <v>352</v>
       </c>
@@ -19024,7 +19024,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="8" s="75" customFormat="1" ht="25" customHeight="1" spans="1:14">
+    <row r="8" s="75" customFormat="1" ht="25" hidden="1" customHeight="1" spans="1:14">
       <c r="A8" s="82" t="s">
         <v>352</v>
       </c>
@@ -19244,7 +19244,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="13" s="78" customFormat="1" ht="25" hidden="1" customHeight="1" spans="1:14">
+    <row r="13" s="78" customFormat="1" ht="25" customHeight="1" spans="1:14">
       <c r="A13" s="94" t="s">
         <v>402</v>
       </c>
@@ -19288,7 +19288,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="14" s="78" customFormat="1" ht="25" hidden="1" customHeight="1" spans="1:14">
+    <row r="14" s="78" customFormat="1" ht="25" customHeight="1" spans="1:14">
       <c r="A14" s="93" t="s">
         <v>402</v>
       </c>
@@ -19332,7 +19332,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="15" s="78" customFormat="1" ht="25" hidden="1" customHeight="1" spans="1:14">
+    <row r="15" s="78" customFormat="1" ht="25" customHeight="1" spans="1:14">
       <c r="A15" s="93" t="s">
         <v>402</v>
       </c>
@@ -19376,7 +19376,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="16" s="78" customFormat="1" ht="25" hidden="1" customHeight="1" spans="1:14">
+    <row r="16" s="78" customFormat="1" ht="25" customHeight="1" spans="1:14">
       <c r="A16" s="93" t="s">
         <v>402</v>
       </c>
@@ -19420,7 +19420,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="17" s="79" customFormat="1" ht="25" hidden="1" customHeight="1" spans="1:14">
+    <row r="17" s="79" customFormat="1" ht="25" customHeight="1" spans="1:14">
       <c r="A17" s="93" t="s">
         <v>402</v>
       </c>
@@ -19464,7 +19464,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="18" s="78" customFormat="1" ht="25" hidden="1" customHeight="1" spans="1:14">
+    <row r="18" s="78" customFormat="1" ht="25" customHeight="1" spans="1:14">
       <c r="A18" s="94" t="s">
         <v>402</v>
       </c>
@@ -19508,7 +19508,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="19" s="78" customFormat="1" ht="25" hidden="1" customHeight="1" spans="1:14">
+    <row r="19" s="78" customFormat="1" ht="25" customHeight="1" spans="1:14">
       <c r="A19" s="94" t="s">
         <v>402</v>
       </c>
@@ -19552,7 +19552,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="20" s="75" customFormat="1" ht="25" customHeight="1" spans="1:14">
+    <row r="20" s="75" customFormat="1" ht="25" hidden="1" customHeight="1" spans="1:14">
       <c r="A20" s="82" t="s">
         <v>352</v>
       </c>
@@ -20264,7 +20264,7 @@
   <autoFilter ref="A2:N34">
     <filterColumn colId="0">
       <customFilters>
-        <customFilter operator="equal" val="Rebeca"/>
+        <customFilter operator="equal" val="Tabita"/>
       </customFilters>
     </filterColumn>
     <extLst/>

</xml_diff>